<commit_message>
continue to next step or schenario if one is empty
</commit_message>
<xml_diff>
--- a/src/main/java/suites/smoke/HyperTech_Automation_Test_Case.xlsx
+++ b/src/main/java/suites/smoke/HyperTech_Automation_Test_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nazmul.islam/Desktop/Personal/HyperTech/ht-selenium-framework/src/main/java/suites/smoke/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C9E19F-1DBC-7F4B-8B2C-54B9C686316A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBFABB2-D2AA-4943-939F-CA923BD5E11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3500" windowWidth="23060" windowHeight="13540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3500" windowWidth="23060" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="1" r:id="rId1"/>
@@ -583,8 +583,8 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>

</xml_diff>